<commit_message>
exp number of benign sources added
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/experiments_traffic.xlsx
+++ b/examples/masterarbeit/experiments_traffic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB05B09-B582-48D4-B252-D21FF4BDB1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD690701-283B-4BC7-AC2F-6640ED0F4522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="36">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>exp_traffic_20191116-142454</t>
+  </si>
+  <si>
+    <t>exp_traffic_20191118-142029</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -760,6 +763,9 @@
       <c r="H10" t="s">
         <v>16</v>
       </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
strange aggregation bug fixed
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/experiments_traffic.xlsx
+++ b/examples/masterarbeit/experiments_traffic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD690701-283B-4BC7-AC2F-6640ED0F4522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EACFA21-9609-455C-942B-D33A5412F00B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="36">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A100B0B-FE3B-4C26-A276-BE253BBFC4CB}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -767,242 +767,239 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5">
         <v>5</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>50</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>64</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s">
-        <v>16</v>
+      <c r="F16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>32</v>
       </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>50</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>50</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0</v>
-      </c>
-      <c r="D21" s="5">
-        <v>64</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5">
         <v>0</v>
@@ -1022,205 +1019,221 @@
       <c r="H23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>64</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="J26" s="5" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>50</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26">
-        <v>100</v>
-      </c>
-      <c r="G26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27">
-        <v>9</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>50</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>64</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28">
         <v>100</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>12</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>50</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30">
-        <v>30</v>
-      </c>
-      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>64</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
         <v>12</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H29" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
         <v>4</v>
       </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>50</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31">
-        <v>50</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
         <v>12</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
         <v>4</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2">
-        <v>50</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>50</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="2">
         <v>100</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>50</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35">
-        <v>50</v>
-      </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="2">
-        <v>4</v>
-      </c>
-      <c r="C36" s="2">
-        <v>1</v>
-      </c>
-      <c r="D36" s="2">
-        <v>50</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2">
-        <v>50</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
@@ -1240,7 +1253,7 @@
         <v>10</v>
       </c>
       <c r="F37">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
@@ -1266,7 +1279,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>12</v>
@@ -1275,61 +1288,61 @@
         <v>15</v>
       </c>
     </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="2">
+      <c r="A40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="2">
         <v>4</v>
       </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2">
-        <v>50</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="2">
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>50</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2">
         <v>100</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>50</v>
-      </c>
-      <c r="E42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42">
-        <v>100</v>
-      </c>
-      <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.4">
@@ -1337,7 +1350,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -1363,7 +1376,7 @@
         <v>9</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1384,13 +1397,65 @@
         <v>16</v>
       </c>
     </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2">
+        <v>9</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>50</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="2">
+        <v>100</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>50</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started with yale experiments
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/experiments_traffic.xlsx
+++ b/examples/masterarbeit/experiments_traffic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB38512-D17B-4550-B323-6B219151988E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE9819-ED7E-4435-8F25-428842567426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="74">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -244,6 +244,15 @@
   </si>
   <si>
     <t>exp_traffic_20200111-183015</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>1,4,5,6,9,10,19,20</t>
+  </si>
+  <si>
+    <t>exp_traffic_20200112-130710</t>
   </si>
 </sst>
 </file>
@@ -681,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A100B0B-FE3B-4C26-A276-BE253BBFC4CB}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -736,8 +745,8 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>72</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -762,9 +771,6 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -785,12 +791,6 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
         <v>64</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>10</v>
       </c>
       <c r="F40">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G40" t="s">
         <v>12</v>
@@ -1595,13 +1595,13 @@
       <c r="H40" t="s">
         <v>15</v>
       </c>
-      <c r="J40" t="s">
-        <v>32</v>
+      <c r="J40" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -1616,21 +1616,17 @@
         <v>10</v>
       </c>
       <c r="F41">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
         <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J41" t="s">
-        <v>60</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L41" s="4"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
@@ -1649,7 +1645,7 @@
         <v>10</v>
       </c>
       <c r="F42">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G42" t="s">
         <v>12</v>
@@ -1658,10 +1654,10 @@
         <v>16</v>
       </c>
       <c r="J42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L42" s="4"/>
     </row>
@@ -1682,7 +1678,7 @@
         <v>10</v>
       </c>
       <c r="F43">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
         <v>12</v>
@@ -1691,79 +1687,84 @@
         <v>16</v>
       </c>
       <c r="J43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="J44"/>
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>64</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L44" s="4"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45"/>
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" t="s">
+        <v>58</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>64</v>
-      </c>
-      <c r="E46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46">
-        <v>50</v>
-      </c>
-      <c r="G46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" t="s">
-        <v>45</v>
-      </c>
+      <c r="J46"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>64</v>
-      </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47">
-        <v>50</v>
-      </c>
-      <c r="G47" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" t="s">
-        <v>38</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="J47"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
@@ -1782,7 +1783,7 @@
         <v>10</v>
       </c>
       <c r="F48">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G48" t="s">
         <v>12</v>
@@ -1791,7 +1792,7 @@
         <v>14</v>
       </c>
       <c r="J48" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
@@ -1811,7 +1812,7 @@
         <v>10</v>
       </c>
       <c r="F49">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G49" t="s">
         <v>12</v>
@@ -1820,87 +1821,82 @@
         <v>15</v>
       </c>
       <c r="J49" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J50"/>
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50">
+        <v>100</v>
+      </c>
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>23</v>
-      </c>
-      <c r="J51"/>
+        <v>8</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>64</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51">
+        <v>100</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52">
-        <v>4</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>64</v>
-      </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52">
-        <v>100</v>
-      </c>
-      <c r="G52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" t="s">
-        <v>15</v>
-      </c>
-      <c r="J52" t="s">
-        <v>32</v>
-      </c>
+      <c r="J52"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53">
-        <v>4</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>64</v>
-      </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53">
-        <v>100</v>
-      </c>
-      <c r="G53" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53" t="str">
-        <f>J43</f>
-        <v>exp_traffic_20191221-160121</v>
-      </c>
-      <c r="K53" s="6" t="str">
-        <f>K43</f>
-        <v>exp_traffic_20191206-151859</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J53"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>8</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1921,7 +1917,7 @@
         <v>15</v>
       </c>
       <c r="J54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.4">
@@ -1929,7 +1925,7 @@
         <v>9</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1949,92 +1945,87 @@
       <c r="H55" t="s">
         <v>16</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" t="str">
+        <f>J45</f>
+        <v>exp_traffic_20191221-160121</v>
+      </c>
+      <c r="K55" s="6" t="str">
+        <f>K45</f>
+        <v>exp_traffic_20191206-151859</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>64</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56">
+        <v>100</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57">
+        <v>100</v>
+      </c>
+      <c r="G57" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" t="s">
         <v>63</v>
       </c>
-      <c r="K55" s="6" t="s">
+      <c r="K57" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J56"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J57"/>
-    </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
         <v>22</v>
       </c>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="2">
-        <v>4</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
-      <c r="D59" s="2">
-        <v>64</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="2">
-        <v>25</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J59" t="str">
-        <f t="shared" ref="J59:K61" si="0">J41</f>
-        <v>exp_traffic_20191222-141343</v>
-      </c>
-      <c r="K59" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>exp_traffic_20191215-151704</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="2">
-        <v>4</v>
-      </c>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2">
-        <v>64</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="2">
-        <v>50</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" t="str">
-        <f t="shared" si="0"/>
-        <v>exp_traffic_20191222-114051</v>
-      </c>
-      <c r="K60" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>exp_traffic_20191209-150036</v>
-      </c>
+      <c r="J60"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
@@ -2053,82 +2044,91 @@
         <v>10</v>
       </c>
       <c r="F61" s="2">
+        <v>25</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" t="str">
+        <f>J42</f>
+        <v>exp_traffic_20191222-141343</v>
+      </c>
+      <c r="K61" s="6" t="str">
+        <f>K42</f>
+        <v>exp_traffic_20191215-151704</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2">
+        <v>64</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="2">
+        <v>50</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" t="str">
+        <f>J43</f>
+        <v>exp_traffic_20191222-114051</v>
+      </c>
+      <c r="K62" s="6" t="str">
+        <f>K43</f>
+        <v>exp_traffic_20191209-150036</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <v>64</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="2">
         <v>100</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J61" t="str">
-        <f t="shared" si="0"/>
+      <c r="G63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" ref="J63:K63" si="0">J45</f>
         <v>exp_traffic_20191221-160121</v>
       </c>
-      <c r="K61" s="6" t="str">
+      <c r="K63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>exp_traffic_20191206-151859</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A62" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="4">
-        <v>4</v>
-      </c>
-      <c r="C62" s="4">
-        <v>1</v>
-      </c>
-      <c r="D62" s="4">
-        <v>64</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="4">
-        <v>12.5</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J62" t="s">
-        <v>54</v>
-      </c>
-      <c r="K62"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A63" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" s="4">
-        <v>4</v>
-      </c>
-      <c r="C63" s="4">
-        <v>1</v>
-      </c>
-      <c r="D63" s="4">
-        <v>64</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" s="4">
-        <v>25</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J63" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
         <v>9</v>
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="F64" s="4">
-        <v>50</v>
+        <v>12.5</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>44</v>
@@ -2155,8 +2155,9 @@
         <v>16</v>
       </c>
       <c r="J64" t="s">
-        <v>53</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K64"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
@@ -2175,7 +2176,7 @@
         <v>10</v>
       </c>
       <c r="F65" s="4">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>44</v>
@@ -2184,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="J65" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.4">
@@ -2204,7 +2205,7 @@
         <v>10</v>
       </c>
       <c r="F66" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>44</v>
@@ -2213,7 +2214,7 @@
         <v>16</v>
       </c>
       <c r="J66" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.4">
@@ -2221,7 +2222,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C67" s="4">
         <v>1</v>
@@ -2233,7 +2234,7 @@
         <v>10</v>
       </c>
       <c r="F67" s="4">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>44</v>
@@ -2242,7 +2243,7 @@
         <v>16</v>
       </c>
       <c r="J67" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.4">
@@ -2250,7 +2251,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C68" s="4">
         <v>1</v>
@@ -2271,6 +2272,64 @@
         <v>16</v>
       </c>
       <c r="J68" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="4">
+        <v>6</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1</v>
+      </c>
+      <c r="D69" s="4">
+        <v>64</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="4">
+        <v>50</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A70" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="4">
+        <v>6</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1</v>
+      </c>
+      <c r="D70" s="4">
+        <v>64</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="4">
+        <v>100</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added many yale experiments
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/experiments_traffic.xlsx
+++ b/examples/masterarbeit/experiments_traffic.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floriannuding/PySyft-fork/examples/masterarbeit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C0265A-7787-104A-A85E-2C09736AF334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619B7DEB-BE10-408E-AF2A-702438CE690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="78">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -246,9 +246,6 @@
     <t>exp_traffic_20200111-183015</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>1,4,5,6,9,10,19,20</t>
   </si>
   <si>
@@ -256,6 +253,18 @@
   </si>
   <si>
     <t>REDO for 100 epochs</t>
+  </si>
+  <si>
+    <t>exp_traffic_20200121-121133</t>
+  </si>
+  <si>
+    <t>exp_traffic_20200124-190249</t>
+  </si>
+  <si>
+    <t>exp_traffic_20200125-083517</t>
+  </si>
+  <si>
+    <t>exp_traffic_20200125-151122</t>
   </si>
 </sst>
 </file>
@@ -701,25 +710,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A100B0B-FE3B-4C26-A276-BE253BBFC4CB}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="30.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="22.5" style="6" customWidth="1"/>
+    <col min="1" max="2" width="15.15234375" customWidth="1"/>
+    <col min="3" max="3" width="16.84375" customWidth="1"/>
+    <col min="5" max="5" width="43.3046875" customWidth="1"/>
+    <col min="6" max="6" width="32.69140625" customWidth="1"/>
+    <col min="7" max="7" width="18.15234375" customWidth="1"/>
+    <col min="8" max="8" width="12.69140625" customWidth="1"/>
+    <col min="10" max="10" width="30.3046875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.4609375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,12 +760,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -777,7 +786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -800,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D4">
         <v>64</v>
       </c>
@@ -811,12 +820,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -845,7 +854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -874,7 +883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -903,7 +912,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -935,7 +944,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -967,7 +976,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1028,16 +1037,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1075,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1106,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1126,7 +1135,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1157,7 +1166,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1186,16 +1195,16 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>18</v>
       </c>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1284,7 +1293,7 @@
       </c>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1324,7 @@
       </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1344,7 +1353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -1357,13 +1366,13 @@
       <c r="J29"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>19</v>
       </c>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1450,7 +1459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1492,7 @@
       </c>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1513,16 +1522,16 @@
       </c>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>20</v>
       </c>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1606,10 +1615,10 @@
         <v>15</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1671,7 +1680,7 @@
       </c>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1713,7 @@
       </c>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1730,11 +1739,11 @@
         <v>16</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1767,16 +1776,16 @@
       </c>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
       <c r="J46"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>24</v>
       </c>
       <c r="J47"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -1863,7 +1872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1892,16 +1901,16 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J52"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>23</v>
       </c>
       <c r="J53"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -1930,7 +1939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>exp_traffic_20191206-151859</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -1993,7 +2002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -2025,19 +2034,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J58"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J59"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>22</v>
       </c>
       <c r="J60"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>9</v>
       </c>
@@ -2071,7 +2080,7 @@
         <v>exp_traffic_20191215-151704</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>9</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>exp_traffic_20191209-150036</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>9</v>
       </c>
@@ -2139,7 +2148,7 @@
         <v>exp_traffic_20191206-151859</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
         <v>9</v>
       </c>
@@ -2169,7 +2178,7 @@
       </c>
       <c r="K64"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
         <v>9</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="s">
         <v>9</v>
       </c>
@@ -2227,10 +2236,10 @@
         <v>53</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A67" s="4" t="s">
         <v>9</v>
       </c>
@@ -2260,7 +2269,7 @@
       </c>
       <c r="K67" s="8"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
         <v>9</v>
       </c>
@@ -2288,11 +2297,11 @@
       <c r="J68" t="s">
         <v>61</v>
       </c>
-      <c r="K68" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K68" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="s">
         <v>9</v>
       </c>
@@ -2320,11 +2329,11 @@
       <c r="J69" t="s">
         <v>65</v>
       </c>
-      <c r="K69" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K69" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A70" s="4" t="s">
         <v>9</v>
       </c>
@@ -2353,7 +2362,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A71" s="4" t="s">
         <v>9</v>
       </c>
@@ -2378,9 +2387,15 @@
       <c r="H71" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J71" s="8" t="s">
-        <v>71</v>
-      </c>
+      <c r="J71" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>